<commit_message>
tamo en el horno
</commit_message>
<xml_diff>
--- a/OBLIGATORIO PARALELO/Lista Funcionalidades Obligatorio Ago 2020 (1).xlsx
+++ b/OBLIGATORIO PARALELO/Lista Funcionalidades Obligatorio Ago 2020 (1).xlsx
@@ -281,14 +281,14 @@
     <t>cuando cambiamos moneda y cambiamos el filtro de ascendente y descendente a la vez ejecuta todo y no por separado</t>
   </si>
   <si>
-    <t xml:space="preserve"> ocultar buscador y cambio de moneda y setear moneda pesos cuando se logea</t>
+    <t>No se está viendo la foto al ver el inmueble registrado y resolver la calificacion para que no aparezca NAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,6 +321,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -371,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -435,7 +441,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -751,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1169,7 +1176,7 @@
       </c>
       <c r="E36" s="21"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="27" t="s">
+      <c r="G36" s="28" t="s">
         <v>84</v>
       </c>
       <c r="H36" s="22"/>
@@ -1318,7 +1325,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="22"/>
     </row>
-    <row r="49" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>51</v>
       </c>
@@ -1331,7 +1338,7 @@
       <c r="H49" s="22"/>
       <c r="I49"/>
     </row>
-    <row r="50" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50"/>
       <c r="B50" s="17" t="s">
         <v>28</v>
@@ -1346,7 +1353,7 @@
       <c r="H50" s="22"/>
       <c r="I50"/>
     </row>
-    <row r="51" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B51" s="14" t="s">
         <v>52</v>
       </c>
@@ -1358,7 +1365,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="22"/>
     </row>
-    <row r="52" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52"/>
       <c r="B52" t="s">
         <v>53</v>
@@ -1373,7 +1380,7 @@
       <c r="H52" s="22"/>
       <c r="I52"/>
     </row>
-    <row r="53" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B53" s="14" t="s">
         <v>54</v>
       </c>
@@ -1385,7 +1392,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="22"/>
     </row>
-    <row r="54" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B54" s="14" t="s">
         <v>55</v>
       </c>
@@ -1397,7 +1404,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="22"/>
     </row>
-    <row r="55" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B55" s="14" t="s">
         <v>56</v>
       </c>
@@ -1409,7 +1416,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="22"/>
     </row>
-    <row r="56" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B56" s="14" t="s">
         <v>57</v>
       </c>
@@ -1421,7 +1428,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="22"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="14"/>
       <c r="B57" s="14" t="s">
         <v>58</v>
@@ -1434,7 +1441,7 @@
       <c r="H57" s="22"/>
       <c r="I57" s="14"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="14"/>
       <c r="B58" s="14" t="s">
         <v>59</v>
@@ -1447,7 +1454,7 @@
       <c r="H58" s="22"/>
       <c r="I58" s="14"/>
     </row>
-    <row r="59" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B59" s="14" t="s">
         <v>60</v>
       </c>
@@ -1459,7 +1466,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="22"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="14"/>
       <c r="B60" s="14" t="s">
         <v>61</v>
@@ -1472,13 +1479,13 @@
       <c r="H60" s="22"/>
       <c r="I60" s="14"/>
     </row>
-    <row r="61" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="2"/>
       <c r="H61" s="22"/>
     </row>
-    <row r="62" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="16" t="s">
         <v>62</v>
       </c>
@@ -1490,7 +1497,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="16"/>
       <c r="B63" s="17" t="s">
         <v>28</v>
@@ -1500,13 +1507,12 @@
         <v>80</v>
       </c>
       <c r="E63" s="21"/>
-      <c r="F63" s="24" t="s">
-        <v>85</v>
-      </c>
+      <c r="F63" s="24"/>
       <c r="G63" s="2"/>
       <c r="H63" s="22"/>
-    </row>
-    <row r="64" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J63" s="27"/>
+    </row>
+    <row r="64" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="16"/>
       <c r="B64" s="17" t="s">
         <v>64</v>
@@ -1594,7 +1600,9 @@
       </c>
       <c r="D70" s="20"/>
       <c r="E70" s="21"/>
-      <c r="F70" s="3"/>
+      <c r="F70" s="24" t="s">
+        <v>85</v>
+      </c>
       <c r="G70" s="2"/>
       <c r="H70" s="22"/>
     </row>

</xml_diff>